<commit_message>
Final Requisitions submitted at 12:30
</commit_message>
<xml_diff>
--- a/Admin/Ganges_Requisitions.xlsx
+++ b/Admin/Ganges_Requisitions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
   <si>
     <t>Column1</t>
   </si>
@@ -98,42 +98,12 @@
     <t>XT60FMPT</t>
   </si>
   <si>
-    <t>Grove - IMU 9DOF v2.0 </t>
-  </si>
-  <si>
-    <t>Cicada 20A BLHeli_S (BB2) 4in1 ESC</t>
-  </si>
-  <si>
-    <t>ED2-C92-645</t>
-  </si>
-  <si>
     <t>EC3 Connectors (Pack of 5)</t>
   </si>
   <si>
     <t>EC3</t>
   </si>
   <si>
-    <t>Maybees</t>
-  </si>
-  <si>
-    <t>IR sensor for proximity</t>
-  </si>
-  <si>
-    <t>SHARP GP2Y0A21YK0F  Distance Measuring Sensor</t>
-  </si>
-  <si>
-    <t>C5D-F21-D1B</t>
-  </si>
-  <si>
-    <t>Supplier: RS components</t>
-  </si>
-  <si>
-    <t>758-9355</t>
-  </si>
-  <si>
-    <t>MicroServo Module</t>
-  </si>
-  <si>
     <t>Supplier: Farnell</t>
   </si>
   <si>
@@ -143,18 +113,6 @@
     <t>Grove - Thumb Joystick</t>
   </si>
   <si>
-    <t>TATTU 1550MAH 11.1V 3S 75C LIPO BATTERY PACK</t>
-  </si>
-  <si>
-    <t>431-B84-06E</t>
-  </si>
-  <si>
-    <t>OLIMEX  OLIMEXINO-32U4  Development Board</t>
-  </si>
-  <si>
-    <t>CHAOS BLHELI_S DSHOT ESC</t>
-  </si>
-  <si>
     <t>B60-1C3-730</t>
   </si>
   <si>
@@ -164,14 +122,38 @@
     <t>TA-45C-1550-3S1P</t>
   </si>
   <si>
-    <t>TATTU 1800MAH 11.1V 3S 45C LIPO BATTERY PACK</t>
+    <t>CHAOS BLHELI_S DSHOT ESC 20A</t>
+  </si>
+  <si>
+    <t>RFM12B-S2 transceiver modules</t>
+  </si>
+  <si>
+    <t>Arduino Leonardo, ATmegaU4</t>
+  </si>
+  <si>
+    <t>SD-Card adaptation for Il Matto</t>
+  </si>
+  <si>
+    <t>Supplier: ECS</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Stripboard</t>
+  </si>
+  <si>
+    <t>LiPo battery charger for 3 cell</t>
+  </si>
+  <si>
+    <t>Various E12 resistors/capacitors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,14 +165,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -221,6 +195,19 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -310,12 +297,12 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -323,17 +310,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -442,6 +436,76 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -464,20 +528,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -500,20 +550,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -536,20 +572,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -572,20 +594,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -605,20 +613,6 @@
         <horizontal style="thin">
           <color auto="1"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -931,12 +925,8 @@
     <tableColumn id="2" name="Column2" dataDxfId="28" totalsRowDxfId="4"/>
     <tableColumn id="3" name="Column3" dataDxfId="27" totalsRowDxfId="3"/>
     <tableColumn id="4" name="Column4" dataDxfId="26" totalsRowDxfId="2"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="1">
-      <totalsRowFormula>SUM(F4:F23,F37:F56,F69:F88)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="6" name="Column6" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="0">
-      <totalsRowFormula>1.2*Table2[[#Totals],[Column5]]</totalsRowFormula>
-    </tableColumn>
+    <tableColumn id="5" name="Column5" dataDxfId="13" totalsRowDxfId="1"/>
+    <tableColumn id="6" name="Column6" dataDxfId="12" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -945,13 +935,16 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="B35:G56" totalsRowShown="0">
   <autoFilter ref="B35:G56"/>
+  <sortState ref="B36:G56">
+    <sortCondition descending="1" ref="B35:B56"/>
+  </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Column1" dataDxfId="23"/>
-    <tableColumn id="2" name="Column2" dataDxfId="22"/>
-    <tableColumn id="3" name="Column3" dataDxfId="21"/>
-    <tableColumn id="4" name="Column4" dataDxfId="20"/>
-    <tableColumn id="5" name="Column5" dataDxfId="19"/>
-    <tableColumn id="6" name="Column6" dataDxfId="18"/>
+    <tableColumn id="1" name="Column1" dataDxfId="25"/>
+    <tableColumn id="2" name="Column2" dataDxfId="24"/>
+    <tableColumn id="3" name="Column3" dataDxfId="23"/>
+    <tableColumn id="4" name="Column4" dataDxfId="22"/>
+    <tableColumn id="5" name="Column5" dataDxfId="21"/>
+    <tableColumn id="6" name="Column6" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -961,12 +954,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="B67:G89" totalsRowCount="1">
   <autoFilter ref="B67:G88"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Column1" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="2" name="Column2" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="3" name="Column3" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="4" name="Column4" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="5" name="Column5" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="6" name="Column6" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="1" name="Column1" dataDxfId="19" totalsRowDxfId="11"/>
+    <tableColumn id="2" name="Column2" dataDxfId="18" totalsRowDxfId="10"/>
+    <tableColumn id="3" name="Column3" dataDxfId="17" totalsRowDxfId="9"/>
+    <tableColumn id="4" name="Column4" dataDxfId="16" totalsRowDxfId="8"/>
+    <tableColumn id="5" name="Column5" dataDxfId="15" totalsRowDxfId="7"/>
+    <tableColumn id="6" name="Column6" dataDxfId="14" totalsRowDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1264,8 +1257,8 @@
   </sheetPr>
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,18 +1273,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1334,356 +1327,290 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>4</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="C4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="7">
         <v>4.99</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <f>Table2[[#This Row],[Column1]]*Table2[[#This Row],[Column4]]</f>
         <v>19.96</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>4.99</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <f>Table2[[#This Row],[Column1]]*Table2[[#This Row],[Column4]]</f>
         <v>9.98</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>2</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>4.99</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <f>Table2[[#This Row],[Column1]]*Table2[[#This Row],[Column4]]</f>
         <v>9.98</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>2</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="8">
+      <c r="C7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="7">
         <v>4.33</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <f>Table2[[#This Row],[Column1]]*Table2[[#This Row],[Column4]]</f>
         <v>8.66</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>1</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>1.04</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <f>Table2[[#This Row],[Column1]]*Table2[[#This Row],[Column4]]</f>
         <v>1.04</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>1</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>0.83</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <f>Table2[[#This Row],[Column1]]*Table2[[#This Row],[Column4]]</f>
         <v>0.83</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>1</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="5">
         <v>2.92</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <f>Table2[[#This Row],[Column1]]*Table2[[#This Row],[Column4]]</f>
         <v>2.92</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>1</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="C11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="5">
         <v>12.49</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <f>Table2[[#This Row],[Column1]]*Table2[[#This Row],[Column4]]</f>
         <v>12.49</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
-        <v>0</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="6">
-        <v>14.16</v>
-      </c>
-      <c r="F12" s="8">
-        <f>Table2[[#This Row],[Column1]]*Table2[[#This Row],[Column4]]</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
-        <v>0</v>
-      </c>
-      <c r="C13" s="6">
-        <v>811003001</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="6">
-        <v>9.33</v>
-      </c>
-      <c r="F13" s="8">
-        <f>Table2[[#This Row],[Column1]]*Table2[[#This Row],[Column4]]</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="8">
-        <v>0</v>
-      </c>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="8">
-        <v>24.99</v>
-      </c>
-      <c r="F14" s="8">
-        <f>Table2[[#This Row],[Column1]]*Table2[[#This Row],[Column4]]</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
-        <v>0</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="6">
-        <v>17.920000000000002</v>
-      </c>
-      <c r="F15" s="6">
-        <f>Table2[[#This Row],[Column1]]*Table2[[#This Row],[Column4]]</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7">
-        <f>SUM(F4:F23,F37:F56,F69:F88)</f>
-        <v>78.959999999999994</v>
-      </c>
-      <c r="G24" s="7">
-        <f>1.2*Table2[[#Totals],[Column5]]</f>
-        <v>94.751999999999995</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F34" s="11"/>
-      <c r="G34" s="12"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="11"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
@@ -1726,204 +1653,191 @@
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="8">
-        <v>0</v>
-      </c>
-      <c r="C37" s="8">
-        <v>1243869</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E37" s="8">
-        <v>5.51</v>
-      </c>
-      <c r="F37" s="4">
-        <f>(Table25[[#This Row],[Column1]]*Table25[[#This Row],[Column4]])</f>
-        <v>0</v>
-      </c>
-      <c r="G37" s="8" t="s">
+      <c r="B37" s="13">
+        <v>1</v>
+      </c>
+      <c r="C37" s="13">
+        <v>2133070</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="13">
+        <v>15.42</v>
+      </c>
+      <c r="F37" s="14">
+        <f>Table25[[#This Row],[Column1]]*Table25[[#This Row],[Column4]]</f>
+        <v>15.42</v>
+      </c>
+      <c r="G37" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="4">
-        <v>1</v>
-      </c>
-      <c r="C38" s="4">
-        <v>2144338</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38" s="4">
-        <v>13.1</v>
-      </c>
-      <c r="F38" s="4">
-        <f>(Table25[[#This Row],[Column1]]*Table25[[#This Row],[Column4]])</f>
-        <v>13.1</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="7"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="4"/>
+      <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="3"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="13"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="3"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="13"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="3"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="13"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="3"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="13"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="3"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="3"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="13"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="3"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="13"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="3"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="13"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C66" s="10"/>
-      <c r="D66" s="5" t="s">
+      <c r="C66" s="9"/>
+      <c r="D66" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E66" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F66" s="11"/>
-      <c r="G66" s="12"/>
+      <c r="E66" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F66" s="10"/>
+      <c r="G66" s="11"/>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
@@ -1966,184 +1880,223 @@
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B69" s="8">
+      <c r="B69" s="13">
+        <v>4</v>
+      </c>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E69" s="13">
+        <v>0</v>
+      </c>
+      <c r="F69" s="13">
+        <f ca="1">Table22[[#This Row],[Column1]]*Table22[[#This Row],[Column5]]</f>
+        <v>0</v>
+      </c>
+      <c r="G69" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="14">
         <v>1</v>
       </c>
-      <c r="C69" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D69" s="8" t="s">
+      <c r="C70" s="14"/>
+      <c r="D70" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E69" s="8">
-        <v>4.71</v>
-      </c>
-      <c r="F69" s="8">
+      <c r="E70" s="14">
         <v>0</v>
       </c>
-      <c r="G69" s="8" t="s">
+      <c r="F70" s="14">
+        <v>0</v>
+      </c>
+      <c r="G70" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-    </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
+      <c r="B71" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E71" s="13">
+        <v>0</v>
+      </c>
+      <c r="F71" s="13">
+        <v>0</v>
+      </c>
+      <c r="G71" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
+      <c r="B72" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E72" s="14">
+        <v>0</v>
+      </c>
+      <c r="F72" s="14">
+        <v>0</v>
+      </c>
+      <c r="G72" s="14" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
+      <c r="B73" s="13">
+        <v>1</v>
+      </c>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E73" s="13">
+        <v>0</v>
+      </c>
+      <c r="F73" s="13">
+        <v>0</v>
+      </c>
+      <c r="G73" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="4"/>
-      <c r="G74" s="4"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
+      <c r="B75" s="13"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="4"/>
-      <c r="G76" s="4"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14"/>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
+      <c r="B77" s="13"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
-      <c r="G78" s="4"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
-      <c r="G80" s="4"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="3"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="14"/>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
+      <c r="B83" s="13"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4"/>
-      <c r="G84" s="4"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="3"/>
+      <c r="B85" s="13"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
+      <c r="B87" s="13"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="14"/>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="7"/>
-      <c r="C89" s="7"/>
-      <c r="D89" s="7"/>
-      <c r="E89" s="7"/>
-      <c r="F89" s="7"/>
-      <c r="G89" s="7"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2154,7 +2107,7 @@
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="E66:G66"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <tableParts count="3">

</xml_diff>